<commit_message>
Update add point/box for template
</commit_message>
<xml_diff>
--- a/src/static/files/order_template.xlsx
+++ b/src/static/files/order_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\py\DJ_Project\src\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69727128-2E47-4C88-A01C-29BBA07A487C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598DB5FC-9A23-40A8-BCD9-E3CCF406ACB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2745" yWindow="2460" windowWidth="14280" windowHeight="8130" xr2:uid="{BE8814AD-4843-489F-99BA-52D0A2E7C26F}"/>
+    <workbookView xWindow="1230" yWindow="1290" windowWidth="21600" windowHeight="11055" xr2:uid="{BE8814AD-4843-489F-99BA-52D0A2E7C26F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t>Mã toa</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>KH240003</t>
+  </si>
+  <si>
+    <t>Điểm 1 thùng</t>
   </si>
 </sst>
 </file>
@@ -241,12 +244,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -268,11 +270,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -588,217 +587,218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2AB322-9057-4DC4-AB23-BED2EFF4F63C}">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1328125" customWidth="1"/>
-    <col min="2" max="2" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.9296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.59765625" customWidth="1"/>
-    <col min="7" max="7" width="12.53125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.9296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.06640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.59765625" customWidth="1"/>
-    <col min="19" max="19" width="12.46484375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="10.5703125" customWidth="1"/>
+    <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A2" s="2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <v>45519</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="5">
+      <c r="I2" s="4">
         <v>45519</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="5">
         <v>300</v>
       </c>
-      <c r="O2" s="7">
+      <c r="O2" s="6">
         <v>20</v>
       </c>
-      <c r="P2" s="6">
+      <c r="P2" s="5">
         <v>66667</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2">
         <f t="shared" ref="Q2:Q3" si="0">N2*P2</f>
         <v>20000100</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A3" s="2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>45526</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>45526</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="5">
         <v>300</v>
       </c>
-      <c r="O3" s="7">
+      <c r="O3" s="6">
         <v>3</v>
       </c>
-      <c r="P3" s="6">
+      <c r="P3" s="5">
         <v>23096</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3">
         <f t="shared" si="0"/>
         <v>6928800</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>45540</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>45540</v>
       </c>
       <c r="J4">
@@ -820,29 +820,29 @@
         <v>2120000</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>45528</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>45528</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" t="s">
         <v>30</v>
       </c>
       <c r="N5">
@@ -857,57 +857,51 @@
       <c r="Q5">
         <v>21200000</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A6" s="2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>8</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>45530</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>45530</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6">
         <v>0</v>
       </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2" t="s">
+      <c r="L6" t="s">
         <v>30</v>
       </c>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2">
+      <c r="N6">
         <v>20</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6">
         <v>1</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6">
         <v>106000</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q6">
         <v>2120000</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R6">
         <v>400000</v>
       </c>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2" t="s">
+      <c r="U6" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>